<commit_message>
add class shopping table
</commit_message>
<xml_diff>
--- a/Curso Excel.xlsx
+++ b/Curso Excel.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Curso Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7A49636-D8AF-48BE-BDB0-2485AD76A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="8_{F7A49636-D8AF-48BE-BDB0-2485AD76A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9AAFE82-CEDB-4B97-9EA1-F800B3E92B25}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{072263F0-9BC5-4A1F-AB46-46643D2FE7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Alunos" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha4" sheetId="4" r:id="rId2"/>
+    <sheet name="Compras" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alunos!$A$1:$D$14</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>NOME</t>
   </si>
@@ -160,13 +160,160 @@
   </si>
   <si>
     <t>COD</t>
+  </si>
+  <si>
+    <t>Luiza Rafhaela</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Ver Série</t>
+  </si>
+  <si>
+    <t>Karla Sued</t>
+  </si>
+  <si>
+    <t>Passear</t>
+  </si>
+  <si>
+    <t>Eliene Querendo</t>
+  </si>
+  <si>
+    <t>Feijoada</t>
+  </si>
+  <si>
+    <t>Contato com Natureza</t>
+  </si>
+  <si>
+    <t>OPERADORES</t>
+  </si>
+  <si>
+    <t>LÓGICOS</t>
+  </si>
+  <si>
+    <t>MATEMÁTICOS</t>
+  </si>
+  <si>
+    <t>FUNÇÕES</t>
+  </si>
+  <si>
+    <t>+ - * /</t>
+  </si>
+  <si>
+    <t>&gt;;&lt;;&gt;=;=;</t>
+  </si>
+  <si>
+    <t>SOMA;</t>
+  </si>
+  <si>
+    <t>TEXTO</t>
+  </si>
+  <si>
+    <t>NÚMERO</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1234456556e</t>
+  </si>
+  <si>
+    <t>(88) 99605-9913</t>
+  </si>
+  <si>
+    <t>123.123.123-12</t>
+  </si>
+  <si>
+    <t>DIFERENTE (&lt;&gt;)</t>
+  </si>
+  <si>
+    <t>PRODUTO</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>QTD</t>
+  </si>
+  <si>
+    <t>PREÇO</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FRALDA</t>
+  </si>
+  <si>
+    <t>FEIJÃO</t>
+  </si>
+  <si>
+    <t>AÇUCAR</t>
+  </si>
+  <si>
+    <t>ARROZ</t>
+  </si>
+  <si>
+    <t>MIOJO</t>
+  </si>
+  <si>
+    <t>CAFÉ</t>
+  </si>
+  <si>
+    <t>SAL</t>
+  </si>
+  <si>
+    <t>LEITE NINHO</t>
+  </si>
+  <si>
+    <t>BULACHA</t>
+  </si>
+  <si>
+    <t>REQUEIJÃO LIGHT</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>MÉDIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +335,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +362,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,10 +417,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -251,6 +469,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,17 +795,18 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -780,6 +1003,48 @@
       </c>
       <c r="D14" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -792,12 +1057,340 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DDE889-A6B8-46F4-B21F-D98B0F8BAFFF}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1796875" customWidth="1"/>
+    <col min="18" max="18" width="13.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <f>C2*D2</f>
+        <v>2</v>
+      </c>
+      <c r="I2" s="6">
+        <v>70</v>
+      </c>
+      <c r="J2" s="6">
+        <v>150</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E11" si="0">C3*D3</f>
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="b">
+        <f>I2&lt;&gt;J2</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <f>I2&gt;J2</f>
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <f>I2&lt;J2</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I4" s="9">
+        <f>I2+J2</f>
+        <v>220</v>
+      </c>
+      <c r="J4" s="9">
+        <f>I2*J2</f>
+        <v>10500</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="11">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5.99</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>29.950000000000003</v>
+      </c>
+      <c r="I5">
+        <f>SUM(I2,J2)</f>
+        <v>220</v>
+      </c>
+      <c r="J5">
+        <f>PRODUCT(I2,J2)</f>
+        <v>10500</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="11">
+        <v>20</v>
+      </c>
+      <c r="D7" s="12">
+        <v>17</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="11">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12">
+        <v>32</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="11">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10">
+        <v>123</v>
+      </c>
+      <c r="I10">
+        <v>123</v>
+      </c>
+      <c r="J10">
+        <v>213</v>
+      </c>
+      <c r="K10">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>9.99</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>39.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="14">
+        <f>SUM(C2:C11)</f>
+        <v>62</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="15">
+        <f>SUM(E2:E11)</f>
+        <v>560.16000000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="15">
+        <f>E12/C12</f>
+        <v>9.0348387096774214</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>